<commit_message>
added new randomised phase files
</commit_message>
<xml_diff>
--- a/xls/correct/G1_LP_A.xlsx
+++ b/xls/correct/G1_LP_A.xlsx
@@ -27,91 +27,91 @@
     <t>ba</t>
   </si>
   <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
     <t>fi</t>
   </si>
   <si>
-    <t>pe</t>
-  </si>
-  <si>
-    <t>pa</t>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>fe</t>
   </si>
   <si>
     <t>we</t>
   </si>
   <si>
+    <t>wa</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
     <t>ta</t>
   </si>
   <si>
-    <t>so</t>
+    <t>te</t>
+  </si>
+  <si>
+    <t>ti</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>ri</t>
   </si>
   <si>
     <t>be</t>
   </si>
   <si>
-    <t>fa</t>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>mi</t>
   </si>
   <si>
     <t>la</t>
   </si>
   <si>
-    <t>fe</t>
-  </si>
-  <si>
-    <t>ni</t>
-  </si>
-  <si>
-    <t>wa</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
-    <t>ki</t>
-  </si>
-  <si>
-    <t>te</t>
-  </si>
-  <si>
-    <t>ka</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>ti</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>po</t>
-  </si>
-  <si>
     <t>le</t>
-  </si>
-  <si>
-    <t>bo</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>mi</t>
-  </si>
-  <si>
-    <t>ri</t>
-  </si>
-  <si>
-    <t>ko</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>to</t>
   </si>
 </sst>
 </file>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,19 +463,19 @@
         <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -510,13 +510,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -545,19 +545,19 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -586,19 +586,19 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
@@ -633,13 +633,13 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
@@ -674,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -709,19 +709,19 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
@@ -750,19 +750,19 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
@@ -791,19 +791,19 @@
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>2</v>
@@ -832,19 +832,19 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -873,19 +873,19 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
         <v>2</v>
@@ -914,19 +914,19 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
         <v>2</v>
@@ -961,13 +961,13 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
         <v>2</v>
@@ -996,7 +996,7 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
         <v>2</v>
@@ -1043,13 +1043,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
@@ -1078,19 +1078,19 @@
         <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
@@ -1125,13 +1125,13 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -1160,19 +1160,19 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
         <v>2</v>
@@ -1207,13 +1207,13 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
@@ -1248,13 +1248,13 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -1283,19 +1283,19 @@
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>2</v>
@@ -1330,13 +1330,13 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s">
         <v>2</v>
@@ -1371,13 +1371,13 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s">
         <v>2</v>
@@ -1406,19 +1406,19 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
         <v>2</v>
@@ -1453,13 +1453,13 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
@@ -1494,13 +1494,13 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
         <v>2</v>
@@ -1529,7 +1529,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
@@ -1576,13 +1576,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
         <v>2</v>
@@ -1617,13 +1617,13 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s">
         <v>2</v>
@@ -1664,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
@@ -1693,19 +1693,19 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
@@ -1746,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
@@ -1775,19 +1775,19 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
         <v>2</v>
@@ -1816,19 +1816,19 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
         <v>2</v>
@@ -1863,13 +1863,13 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
         <v>2</v>
@@ -1904,13 +1904,13 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
         <v>2</v>
@@ -1939,19 +1939,19 @@
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
         <v>2</v>
@@ -1986,13 +1986,13 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
         <v>2</v>
@@ -2027,13 +2027,13 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
         <v>2</v>
@@ -2062,19 +2062,19 @@
         <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
changed gfx size, enable all keys, correct LP phases (resorted)
</commit_message>
<xml_diff>
--- a/xls/correct/G1_LP_A.xlsx
+++ b/xls/correct/G1_LP_A.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="10050"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,22 +747,22 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -829,22 +829,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -920,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -1034,22 +1034,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>2</v>
@@ -1075,22 +1075,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
@@ -1116,22 +1116,22 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -1157,22 +1157,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
         <v>2</v>
@@ -1198,22 +1198,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1289,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1330,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -1362,22 +1362,22 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
         <v>2</v>
@@ -1403,22 +1403,22 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
         <v>2</v>
@@ -1444,22 +1444,22 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
@@ -1649,22 +1649,22 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
@@ -1690,22 +1690,22 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
@@ -1731,22 +1731,22 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
@@ -1772,22 +1772,22 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
         <v>2</v>

</xml_diff>